<commit_message>
Daily Commit Tag 3 10.03.2022
added Projekt cambotmanager
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
+++ b/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\Alles IPA\Git\Cambotmanager-IPA-Maurice-Meier\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076B9604-B690-421B-846A-D40C1F7CCD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549B3338-5918-4F17-9CBC-21CB42B6878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Arbeiten</t>
   </si>
@@ -118,14 +118,20 @@
     <t>1h</t>
   </si>
   <si>
-    <t>s</t>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>1,5h</t>
+  </si>
+  <si>
+    <t>2,5h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +161,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -712,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -768,6 +781,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -778,6 +794,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -813,24 +844,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1152,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D82CD-F568-433E-90D3-FE24E407675F}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,59 +1394,59 @@
     <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="61" t="s">
+      <c r="D7" s="69"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="62"/>
-      <c r="H7" s="61" t="s">
+      <c r="G7" s="70"/>
+      <c r="H7" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="61" t="s">
+      <c r="I7" s="70"/>
+      <c r="J7" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="62"/>
-      <c r="L7" s="61" t="s">
+      <c r="K7" s="70"/>
+      <c r="L7" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="62"/>
-      <c r="N7" s="61" t="s">
+      <c r="M7" s="70"/>
+      <c r="N7" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="62"/>
-      <c r="P7" s="61" t="s">
+      <c r="O7" s="70"/>
+      <c r="P7" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="61" t="s">
+      <c r="Q7" s="70"/>
+      <c r="R7" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="62"/>
-      <c r="T7" s="61" t="s">
+      <c r="S7" s="70"/>
+      <c r="T7" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="62"/>
-      <c r="V7" s="61" t="s">
+      <c r="U7" s="70"/>
+      <c r="V7" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="W7" s="62"/>
-      <c r="X7" s="61" t="s">
+      <c r="W7" s="70"/>
+      <c r="X7" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="62"/>
-      <c r="Z7" s="61" t="s">
+      <c r="Y7" s="70"/>
+      <c r="Z7" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="61" t="s">
+      <c r="AA7" s="70"/>
+      <c r="AB7" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="AC7" s="62"/>
+      <c r="AC7" s="70"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
@@ -1435,33 +1455,33 @@
     <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="64"/>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="63"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="63"/>
-      <c r="W8" s="64"/>
-      <c r="X8" s="63"/>
-      <c r="Y8" s="64"/>
-      <c r="Z8" s="63"/>
-      <c r="AA8" s="64"/>
-      <c r="AB8" s="63"/>
-      <c r="AC8" s="64"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="72"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="72"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="72"/>
+      <c r="Z8" s="71"/>
+      <c r="AA8" s="72"/>
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="72"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -1470,10 +1490,10 @@
     <row r="9" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="69"/>
+      <c r="D9" s="77"/>
       <c r="E9" s="9" t="s">
         <v>2</v>
       </c>
@@ -1509,8 +1529,8 @@
     <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
       <c r="E10" s="14" t="s">
         <v>3</v>
       </c>
@@ -1546,10 +1566,10 @@
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="56"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="18" t="s">
         <v>2</v>
       </c>
@@ -1585,8 +1605,8 @@
     <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
       <c r="E12" s="22" t="s">
         <v>3</v>
       </c>
@@ -1596,7 +1616,9 @@
         <v>26</v>
       </c>
       <c r="I12" s="28"/>
-      <c r="J12" s="48"/>
+      <c r="J12" s="78" t="s">
+        <v>28</v>
+      </c>
       <c r="K12" s="16"/>
       <c r="L12" s="48"/>
       <c r="M12" s="16"/>
@@ -1624,10 +1646,10 @@
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="56"/>
+      <c r="D13" s="59"/>
       <c r="E13" s="18" t="s">
         <v>2</v>
       </c>
@@ -1663,8 +1685,8 @@
     <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="61"/>
       <c r="E14" s="22" t="s">
         <v>3</v>
       </c>
@@ -1673,7 +1695,9 @@
       <c r="H14" s="42"/>
       <c r="I14" s="17"/>
       <c r="J14" s="48"/>
-      <c r="K14" s="16"/>
+      <c r="K14" s="79" t="s">
+        <v>27</v>
+      </c>
       <c r="L14" s="48"/>
       <c r="M14" s="16"/>
       <c r="N14" s="48"/>
@@ -1700,10 +1724,10 @@
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="59"/>
       <c r="E15" s="18" t="s">
         <v>2</v>
       </c>
@@ -1711,8 +1735,8 @@
       <c r="G15" s="41"/>
       <c r="H15" s="41"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="19"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="82"/>
       <c r="L15" s="50"/>
       <c r="M15" s="21"/>
       <c r="N15" s="49"/>
@@ -1739,8 +1763,8 @@
     <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="61"/>
       <c r="E16" s="22" t="s">
         <v>3</v>
       </c>
@@ -1748,8 +1772,8 @@
       <c r="G16" s="42"/>
       <c r="H16" s="54"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="16"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="84"/>
       <c r="L16" s="48"/>
       <c r="M16" s="16"/>
       <c r="N16" s="48"/>
@@ -1776,8 +1800,8 @@
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="56" t="s">
+      <c r="C17" s="63"/>
+      <c r="D17" s="59" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="18" t="s">
@@ -1815,8 +1839,8 @@
     <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="74"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="66"/>
       <c r="E18" s="22" t="s">
         <v>3</v>
       </c>
@@ -1824,8 +1848,10 @@
       <c r="G18" s="42"/>
       <c r="H18" s="42"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="16"/>
+      <c r="J18" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="79"/>
       <c r="L18" s="48"/>
       <c r="M18" s="16"/>
       <c r="N18" s="48"/>
@@ -1852,8 +1878,8 @@
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="56" t="s">
+      <c r="C19" s="64"/>
+      <c r="D19" s="59" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="18" t="s">
@@ -1891,8 +1917,8 @@
     <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="74"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="22" t="s">
         <v>3</v>
       </c>
@@ -1928,8 +1954,8 @@
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="56" t="s">
+      <c r="C21" s="64"/>
+      <c r="D21" s="59" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="30" t="s">
@@ -1967,8 +1993,8 @@
     <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="74"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
       <c r="E22" s="31" t="s">
         <v>3</v>
       </c>
@@ -2004,10 +2030,10 @@
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="56"/>
+      <c r="D23" s="59"/>
       <c r="E23" s="18" t="s">
         <v>2</v>
       </c>
@@ -2043,8 +2069,8 @@
     <row r="24" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="61"/>
       <c r="E24" s="22" t="s">
         <v>3</v>
       </c>
@@ -2080,10 +2106,10 @@
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="56"/>
+      <c r="D25" s="59"/>
       <c r="E25" s="18" t="s">
         <v>2</v>
       </c>
@@ -2119,8 +2145,8 @@
     <row r="26" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="61"/>
       <c r="E26" s="22" t="s">
         <v>3</v>
       </c>
@@ -2156,10 +2182,10 @@
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="56"/>
+      <c r="D27" s="59"/>
       <c r="E27" s="18" t="s">
         <v>2</v>
       </c>
@@ -2195,13 +2221,13 @@
     <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="68"/>
       <c r="E28" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F28" s="27"/>
-      <c r="G28" s="76"/>
+      <c r="G28" s="56"/>
       <c r="H28" s="46"/>
       <c r="I28" s="25"/>
       <c r="J28" s="52"/>
@@ -2377,9 +2403,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="2"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="H33" s="7"/>
       <c r="I33" s="4"/>
       <c r="J33" s="8"/>
       <c r="K33" s="4"/>
@@ -2387,7 +2411,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="75"/>
+      <c r="P33" s="55"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
@@ -2837,7 +2861,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="77"/>
+      <c r="I46" s="57"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2897,14 +2921,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C25:D26"/>
     <mergeCell ref="C27:D28"/>
     <mergeCell ref="AB7:AC8"/>
@@ -2921,6 +2937,14 @@
     <mergeCell ref="L7:M8"/>
     <mergeCell ref="N7:O8"/>
     <mergeCell ref="C9:D10"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Daily Commit 11.03.2022 / Tag 4
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
+++ b/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\Alles IPA\Git\Cambotmanager-IPA-Maurice-Meier\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549B3338-5918-4F17-9CBC-21CB42B6878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF16B41A-11C3-4C77-B0FE-624B1F6E0245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Arbeiten</t>
   </si>
@@ -725,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -784,6 +784,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,21 +801,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -844,13 +836,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1172,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D82CD-F568-433E-90D3-FE24E407675F}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,59 +1395,59 @@
     <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="69" t="s">
+      <c r="D7" s="71"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="70"/>
-      <c r="H7" s="69" t="s">
+      <c r="G7" s="72"/>
+      <c r="H7" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="70"/>
-      <c r="J7" s="69" t="s">
+      <c r="I7" s="72"/>
+      <c r="J7" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="70"/>
-      <c r="L7" s="69" t="s">
+      <c r="K7" s="72"/>
+      <c r="L7" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="70"/>
-      <c r="N7" s="69" t="s">
+      <c r="M7" s="72"/>
+      <c r="N7" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="70"/>
-      <c r="P7" s="69" t="s">
+      <c r="O7" s="72"/>
+      <c r="P7" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="69" t="s">
+      <c r="Q7" s="72"/>
+      <c r="R7" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="70"/>
-      <c r="T7" s="69" t="s">
+      <c r="S7" s="72"/>
+      <c r="T7" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="70"/>
-      <c r="V7" s="69" t="s">
+      <c r="U7" s="72"/>
+      <c r="V7" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="W7" s="70"/>
-      <c r="X7" s="69" t="s">
+      <c r="W7" s="72"/>
+      <c r="X7" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="70"/>
-      <c r="Z7" s="69" t="s">
+      <c r="Y7" s="72"/>
+      <c r="Z7" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="AA7" s="70"/>
-      <c r="AB7" s="69" t="s">
+      <c r="AA7" s="72"/>
+      <c r="AB7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="AC7" s="70"/>
+      <c r="AC7" s="72"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
@@ -1455,33 +1456,33 @@
     <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="71"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="71"/>
-      <c r="U8" s="72"/>
-      <c r="V8" s="71"/>
-      <c r="W8" s="72"/>
-      <c r="X8" s="71"/>
-      <c r="Y8" s="72"/>
-      <c r="Z8" s="71"/>
-      <c r="AA8" s="72"/>
-      <c r="AB8" s="71"/>
-      <c r="AC8" s="72"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="73"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="73"/>
+      <c r="AC8" s="74"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -1490,10 +1491,10 @@
     <row r="9" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="77"/>
+      <c r="D9" s="79"/>
       <c r="E9" s="9" t="s">
         <v>2</v>
       </c>
@@ -1529,8 +1530,8 @@
     <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="14" t="s">
         <v>3</v>
       </c>
@@ -1566,10 +1567,10 @@
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="59"/>
+      <c r="D11" s="66"/>
       <c r="E11" s="18" t="s">
         <v>2</v>
       </c>
@@ -1605,8 +1606,8 @@
     <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="22" t="s">
         <v>3</v>
       </c>
@@ -1616,12 +1617,14 @@
         <v>26</v>
       </c>
       <c r="I12" s="28"/>
-      <c r="J12" s="78" t="s">
+      <c r="J12" s="58" t="s">
         <v>28</v>
       </c>
       <c r="K12" s="16"/>
       <c r="L12" s="48"/>
-      <c r="M12" s="16"/>
+      <c r="M12" s="59" t="s">
+        <v>27</v>
+      </c>
       <c r="N12" s="48"/>
       <c r="O12" s="16"/>
       <c r="P12" s="48"/>
@@ -1646,10 +1649,10 @@
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="59"/>
+      <c r="D13" s="66"/>
       <c r="E13" s="18" t="s">
         <v>2</v>
       </c>
@@ -1685,8 +1688,8 @@
     <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="61"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="22" t="s">
         <v>3</v>
       </c>
@@ -1695,7 +1698,7 @@
       <c r="H14" s="42"/>
       <c r="I14" s="17"/>
       <c r="J14" s="48"/>
-      <c r="K14" s="79" t="s">
+      <c r="K14" s="59" t="s">
         <v>27</v>
       </c>
       <c r="L14" s="48"/>
@@ -1724,10 +1727,10 @@
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="59"/>
+      <c r="D15" s="66"/>
       <c r="E15" s="18" t="s">
         <v>2</v>
       </c>
@@ -1735,8 +1738,8 @@
       <c r="G15" s="41"/>
       <c r="H15" s="41"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="82"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
       <c r="L15" s="50"/>
       <c r="M15" s="21"/>
       <c r="N15" s="49"/>
@@ -1763,8 +1766,8 @@
     <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="22" t="s">
         <v>3</v>
       </c>
@@ -1772,8 +1775,8 @@
       <c r="G16" s="42"/>
       <c r="H16" s="54"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="84"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="64"/>
       <c r="L16" s="48"/>
       <c r="M16" s="16"/>
       <c r="N16" s="48"/>
@@ -1800,8 +1803,8 @@
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="59" t="s">
+      <c r="C17" s="81"/>
+      <c r="D17" s="66" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="18" t="s">
@@ -1839,8 +1842,8 @@
     <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="66"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="84"/>
       <c r="E18" s="22" t="s">
         <v>3</v>
       </c>
@@ -1848,12 +1851,12 @@
       <c r="G18" s="42"/>
       <c r="H18" s="42"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="80" t="s">
+      <c r="J18" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="79"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="16"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="59"/>
       <c r="N18" s="48"/>
       <c r="O18" s="16"/>
       <c r="P18" s="48"/>
@@ -1878,8 +1881,8 @@
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="59" t="s">
+      <c r="C19" s="82"/>
+      <c r="D19" s="66" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="18" t="s">
@@ -1917,8 +1920,8 @@
     <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="66"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="84"/>
       <c r="E20" s="22" t="s">
         <v>3</v>
       </c>
@@ -1954,8 +1957,8 @@
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="59" t="s">
+      <c r="C21" s="82"/>
+      <c r="D21" s="66" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="30" t="s">
@@ -1993,8 +1996,8 @@
     <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="84"/>
       <c r="E22" s="31" t="s">
         <v>3</v>
       </c>
@@ -2030,10 +2033,10 @@
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="59"/>
+      <c r="D23" s="66"/>
       <c r="E23" s="18" t="s">
         <v>2</v>
       </c>
@@ -2069,8 +2072,8 @@
     <row r="24" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="61"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="68"/>
       <c r="E24" s="22" t="s">
         <v>3</v>
       </c>
@@ -2106,10 +2109,10 @@
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="58" t="s">
+      <c r="C25" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="59"/>
+      <c r="D25" s="66"/>
       <c r="E25" s="18" t="s">
         <v>2</v>
       </c>
@@ -2145,8 +2148,8 @@
     <row r="26" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="61"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="68"/>
       <c r="E26" s="22" t="s">
         <v>3</v>
       </c>
@@ -2182,10 +2185,10 @@
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="59"/>
+      <c r="D27" s="66"/>
       <c r="E27" s="18" t="s">
         <v>2</v>
       </c>
@@ -2221,8 +2224,8 @@
     <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="68"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="23" t="s">
         <v>3</v>
       </c>
@@ -2231,7 +2234,7 @@
       <c r="H28" s="46"/>
       <c r="I28" s="25"/>
       <c r="J28" s="52"/>
-      <c r="K28" s="24"/>
+      <c r="K28" s="85"/>
       <c r="L28" s="52"/>
       <c r="M28" s="24"/>
       <c r="N28" s="52"/>
@@ -2921,6 +2924,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C25:D26"/>
     <mergeCell ref="C27:D28"/>
     <mergeCell ref="AB7:AC8"/>
@@ -2937,14 +2948,6 @@
     <mergeCell ref="L7:M8"/>
     <mergeCell ref="N7:O8"/>
     <mergeCell ref="C9:D10"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Daily Commit 16.03.2022 Tag 6
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
+++ b/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\Alles IPA\Git\Cambotmanager-IPA-Maurice-Meier\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF16B41A-11C3-4C77-B0FE-624B1F6E0245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2638467D-F386-4739-B944-0D5BDC80FF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
-  <si>
-    <t>Arbeiten</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>07.03.2022</t>
   </si>
@@ -125,6 +122,12 @@
   </si>
   <si>
     <t>2,5h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Tätigkeit</t>
   </si>
 </sst>
 </file>
@@ -725,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -791,6 +794,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -801,6 +806,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -836,21 +856,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D82CD-F568-433E-90D3-FE24E407675F}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,59 +1401,59 @@
     <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="78"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="72"/>
-      <c r="H7" s="71" t="s">
+      <c r="G7" s="79"/>
+      <c r="H7" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="79"/>
+      <c r="J7" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="72"/>
-      <c r="J7" s="71" t="s">
+      <c r="K7" s="79"/>
+      <c r="L7" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="72"/>
-      <c r="L7" s="71" t="s">
+      <c r="M7" s="79"/>
+      <c r="N7" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="72"/>
-      <c r="N7" s="71" t="s">
+      <c r="O7" s="79"/>
+      <c r="P7" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="72"/>
-      <c r="P7" s="71" t="s">
+      <c r="Q7" s="79"/>
+      <c r="R7" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="72"/>
-      <c r="R7" s="71" t="s">
+      <c r="S7" s="79"/>
+      <c r="T7" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="72"/>
-      <c r="T7" s="71" t="s">
+      <c r="U7" s="79"/>
+      <c r="V7" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="72"/>
-      <c r="V7" s="71" t="s">
+      <c r="W7" s="79"/>
+      <c r="X7" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="W7" s="72"/>
-      <c r="X7" s="71" t="s">
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="72"/>
-      <c r="Z7" s="71" t="s">
+      <c r="AA7" s="79"/>
+      <c r="AB7" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="AA7" s="72"/>
-      <c r="AB7" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC7" s="72"/>
+      <c r="AC7" s="79"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
@@ -1456,33 +1462,33 @@
     <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="74"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="73"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="73"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="73"/>
-      <c r="AA8" s="74"/>
-      <c r="AB8" s="73"/>
-      <c r="AC8" s="74"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="80"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="80"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="80"/>
+      <c r="Y8" s="81"/>
+      <c r="Z8" s="80"/>
+      <c r="AA8" s="81"/>
+      <c r="AB8" s="80"/>
+      <c r="AC8" s="81"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -1491,12 +1497,12 @@
     <row r="9" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="78" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="79"/>
+      <c r="C9" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="86"/>
       <c r="E9" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="39"/>
@@ -1530,10 +1536,10 @@
     <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="68"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="26"/>
       <c r="G10" s="40"/>
@@ -1541,7 +1547,9 @@
       <c r="I10" s="17"/>
       <c r="J10" s="48"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="48"/>
+      <c r="L10" s="60" t="s">
+        <v>26</v>
+      </c>
       <c r="M10" s="16"/>
       <c r="N10" s="48"/>
       <c r="O10" s="16"/>
@@ -1567,12 +1575,12 @@
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="66"/>
+      <c r="C11" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="68"/>
       <c r="E11" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="41"/>
@@ -1606,25 +1614,23 @@
     <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="68"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="42"/>
       <c r="H12" s="40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="28"/>
       <c r="J12" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12" s="16"/>
       <c r="L12" s="48"/>
-      <c r="M12" s="59" t="s">
-        <v>27</v>
-      </c>
+      <c r="M12" s="16"/>
       <c r="N12" s="48"/>
       <c r="O12" s="16"/>
       <c r="P12" s="48"/>
@@ -1649,12 +1655,12 @@
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="66"/>
+      <c r="C13" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="68"/>
       <c r="E13" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="41"/>
@@ -1688,10 +1694,10 @@
     <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
       <c r="E14" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="42"/>
@@ -1699,7 +1705,7 @@
       <c r="I14" s="17"/>
       <c r="J14" s="48"/>
       <c r="K14" s="59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L14" s="48"/>
       <c r="M14" s="16"/>
@@ -1727,12 +1733,12 @@
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="66"/>
+      <c r="C15" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="68"/>
       <c r="E15" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="41"/>
@@ -1766,10 +1772,10 @@
     <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="70"/>
       <c r="E16" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="42"/>
@@ -1803,12 +1809,12 @@
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="66" t="s">
-        <v>23</v>
+      <c r="C17" s="72"/>
+      <c r="D17" s="68" t="s">
+        <v>22</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="41"/>
@@ -1842,24 +1848,26 @@
     <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="84"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="42"/>
       <c r="H18" s="42"/>
       <c r="I18" s="17"/>
       <c r="J18" s="60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K18" s="59"/>
       <c r="L18" s="60"/>
       <c r="M18" s="59"/>
-      <c r="N18" s="48"/>
+      <c r="N18" s="60"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="48"/>
+      <c r="P18" s="60" t="s">
+        <v>25</v>
+      </c>
       <c r="Q18" s="17"/>
       <c r="R18" s="48"/>
       <c r="S18" s="16"/>
@@ -1881,12 +1889,12 @@
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="66" t="s">
-        <v>24</v>
+      <c r="C19" s="73"/>
+      <c r="D19" s="68" t="s">
+        <v>23</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="41"/>
@@ -1920,10 +1928,10 @@
     <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="84"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="75"/>
       <c r="E20" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="41"/>
@@ -1934,8 +1942,10 @@
       <c r="L20" s="50"/>
       <c r="M20" s="19"/>
       <c r="N20" s="50"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="50"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="66" t="s">
+        <v>29</v>
+      </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="50"/>
       <c r="S20" s="19"/>
@@ -1957,12 +1967,12 @@
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="66" t="s">
-        <v>25</v>
+      <c r="C21" s="73"/>
+      <c r="D21" s="68" t="s">
+        <v>24</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="43"/>
@@ -1996,10 +2006,10 @@
     <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="84"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" s="37"/>
       <c r="G22" s="42"/>
@@ -2033,12 +2043,12 @@
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="66"/>
+      <c r="C23" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="68"/>
       <c r="E23" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="41"/>
@@ -2072,10 +2082,10 @@
     <row r="24" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
       <c r="E24" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="42"/>
@@ -2109,12 +2119,12 @@
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="66"/>
+      <c r="C25" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="68"/>
       <c r="E25" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="41"/>
@@ -2148,10 +2158,10 @@
     <row r="26" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="68"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="70"/>
       <c r="E26" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="42"/>
@@ -2185,12 +2195,12 @@
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="66"/>
+      <c r="C27" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="68"/>
       <c r="E27" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="44"/>
@@ -2224,22 +2234,26 @@
     <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="70"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="77"/>
       <c r="E28" s="23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="56"/>
       <c r="H28" s="46"/>
       <c r="I28" s="25"/>
       <c r="J28" s="52"/>
-      <c r="K28" s="85"/>
+      <c r="K28" s="88" t="s">
+        <v>26</v>
+      </c>
       <c r="L28" s="52"/>
       <c r="M28" s="24"/>
       <c r="N28" s="52"/>
       <c r="O28" s="24"/>
-      <c r="P28" s="52"/>
+      <c r="P28" s="87" t="s">
+        <v>25</v>
+      </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="52"/>
       <c r="S28" s="24"/>
@@ -2440,15 +2454,15 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -2924,14 +2938,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C25:D26"/>
     <mergeCell ref="C27:D28"/>
     <mergeCell ref="AB7:AC8"/>
@@ -2948,6 +2954,14 @@
     <mergeCell ref="L7:M8"/>
     <mergeCell ref="N7:O8"/>
     <mergeCell ref="C9:D10"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ready for test on raspberry
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
+++ b/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\Alles IPA\Git\Cambotmanager-IPA-Maurice-Meier\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2638467D-F386-4739-B944-0D5BDC80FF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B38945-DA68-42A6-B350-484770149E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -796,6 +796,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,21 +808,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -856,8 +843,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:AG50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,59 +1401,59 @@
     <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="78"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="78" t="s">
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="79"/>
-      <c r="H7" s="78" t="s">
+      <c r="G7" s="76"/>
+      <c r="H7" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="78" t="s">
+      <c r="I7" s="76"/>
+      <c r="J7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="79"/>
-      <c r="L7" s="78" t="s">
+      <c r="K7" s="76"/>
+      <c r="L7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="79"/>
-      <c r="N7" s="78" t="s">
+      <c r="M7" s="76"/>
+      <c r="N7" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="79"/>
-      <c r="P7" s="78" t="s">
+      <c r="O7" s="76"/>
+      <c r="P7" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="78" t="s">
+      <c r="Q7" s="76"/>
+      <c r="R7" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="S7" s="79"/>
-      <c r="T7" s="78" t="s">
+      <c r="S7" s="76"/>
+      <c r="T7" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="79"/>
-      <c r="V7" s="78" t="s">
+      <c r="U7" s="76"/>
+      <c r="V7" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="W7" s="79"/>
-      <c r="X7" s="78" t="s">
+      <c r="W7" s="76"/>
+      <c r="X7" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="79"/>
-      <c r="Z7" s="78" t="s">
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="AA7" s="79"/>
-      <c r="AB7" s="78" t="s">
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="AC7" s="79"/>
+      <c r="AC7" s="76"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
@@ -1462,33 +1462,33 @@
     <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="80"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="80"/>
-      <c r="S8" s="81"/>
-      <c r="T8" s="80"/>
-      <c r="U8" s="81"/>
-      <c r="V8" s="80"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="80"/>
-      <c r="Y8" s="81"/>
-      <c r="Z8" s="80"/>
-      <c r="AA8" s="81"/>
-      <c r="AB8" s="80"/>
-      <c r="AC8" s="81"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="77"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="78"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="78"/>
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="78"/>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="78"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -1497,10 +1497,10 @@
     <row r="9" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="86"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="9" t="s">
         <v>1</v>
       </c>
@@ -1536,8 +1536,8 @@
     <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="70"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="14" t="s">
         <v>2</v>
       </c>
@@ -1575,10 +1575,10 @@
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="68"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="18" t="s">
         <v>1</v>
       </c>
@@ -1614,8 +1614,8 @@
     <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="22" t="s">
         <v>2</v>
       </c>
@@ -1655,10 +1655,10 @@
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="68"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="18" t="s">
         <v>1</v>
       </c>
@@ -1694,8 +1694,8 @@
     <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="70"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="22" t="s">
         <v>2</v>
       </c>
@@ -1733,10 +1733,10 @@
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="68"/>
+      <c r="D15" s="70"/>
       <c r="E15" s="18" t="s">
         <v>1</v>
       </c>
@@ -1772,8 +1772,8 @@
     <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="70"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="22" t="s">
         <v>2</v>
       </c>
@@ -1809,8 +1809,8 @@
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="68" t="s">
+      <c r="C17" s="85"/>
+      <c r="D17" s="70" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="18" t="s">
@@ -1848,8 +1848,8 @@
     <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="75"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="22" t="s">
         <v>2</v>
       </c>
@@ -1889,8 +1889,8 @@
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="68" t="s">
+      <c r="C19" s="86"/>
+      <c r="D19" s="70" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="18" t="s">
@@ -1928,8 +1928,8 @@
     <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="75"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="88"/>
       <c r="E20" s="22" t="s">
         <v>2</v>
       </c>
@@ -1967,8 +1967,8 @@
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="68" t="s">
+      <c r="C21" s="86"/>
+      <c r="D21" s="70" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="30" t="s">
@@ -2006,8 +2006,8 @@
     <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="75"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="88"/>
       <c r="E22" s="31" t="s">
         <v>2</v>
       </c>
@@ -2043,10 +2043,10 @@
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="68"/>
+      <c r="D23" s="70"/>
       <c r="E23" s="18" t="s">
         <v>1</v>
       </c>
@@ -2082,8 +2082,8 @@
     <row r="24" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="70"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="72"/>
       <c r="E24" s="22" t="s">
         <v>2</v>
       </c>
@@ -2119,10 +2119,10 @@
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="68"/>
+      <c r="D25" s="70"/>
       <c r="E25" s="18" t="s">
         <v>1</v>
       </c>
@@ -2158,8 +2158,8 @@
     <row r="26" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="70"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="22" t="s">
         <v>2</v>
       </c>
@@ -2195,10 +2195,10 @@
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="68"/>
+      <c r="D27" s="70"/>
       <c r="E27" s="18" t="s">
         <v>1</v>
       </c>
@@ -2234,8 +2234,8 @@
     <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="77"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="74"/>
       <c r="E28" s="23" t="s">
         <v>2</v>
       </c>
@@ -2244,14 +2244,14 @@
       <c r="H28" s="46"/>
       <c r="I28" s="25"/>
       <c r="J28" s="52"/>
-      <c r="K28" s="88" t="s">
+      <c r="K28" s="68" t="s">
         <v>26</v>
       </c>
       <c r="L28" s="52"/>
       <c r="M28" s="24"/>
       <c r="N28" s="52"/>
       <c r="O28" s="24"/>
-      <c r="P28" s="87" t="s">
+      <c r="P28" s="67" t="s">
         <v>25</v>
       </c>
       <c r="Q28" s="25"/>
@@ -2938,6 +2938,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C25:D26"/>
     <mergeCell ref="C27:D28"/>
     <mergeCell ref="AB7:AC8"/>
@@ -2954,14 +2962,6 @@
     <mergeCell ref="L7:M8"/>
     <mergeCell ref="N7:O8"/>
     <mergeCell ref="C9:D10"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Daily Comit 18.03.2022 / Tag 8
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
+++ b/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\Alles IPA\Git\Cambotmanager-IPA-Maurice-Meier\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B38945-DA68-42A6-B350-484770149E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF59255-8E1D-4990-8CA5-DD5F23475073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>07.03.2022</t>
   </si>
@@ -728,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -810,6 +810,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -843,21 +858,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1179,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D82CD-F568-433E-90D3-FE24E407675F}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,59 +1403,59 @@
     <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="75" t="s">
+      <c r="D7" s="80"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="75" t="s">
+      <c r="G7" s="81"/>
+      <c r="H7" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="75" t="s">
+      <c r="I7" s="81"/>
+      <c r="J7" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="75" t="s">
+      <c r="K7" s="81"/>
+      <c r="L7" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="76"/>
-      <c r="N7" s="75" t="s">
+      <c r="M7" s="81"/>
+      <c r="N7" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="76"/>
-      <c r="P7" s="75" t="s">
+      <c r="O7" s="81"/>
+      <c r="P7" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="75" t="s">
+      <c r="Q7" s="81"/>
+      <c r="R7" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="S7" s="76"/>
-      <c r="T7" s="75" t="s">
+      <c r="S7" s="81"/>
+      <c r="T7" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="76"/>
-      <c r="V7" s="75" t="s">
+      <c r="U7" s="81"/>
+      <c r="V7" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="W7" s="76"/>
-      <c r="X7" s="75" t="s">
+      <c r="W7" s="81"/>
+      <c r="X7" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="76"/>
-      <c r="Z7" s="75" t="s">
+      <c r="Y7" s="81"/>
+      <c r="Z7" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="AA7" s="76"/>
-      <c r="AB7" s="75" t="s">
+      <c r="AA7" s="81"/>
+      <c r="AB7" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="AC7" s="76"/>
+      <c r="AC7" s="81"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
@@ -1462,33 +1464,33 @@
     <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
-      <c r="X8" s="77"/>
-      <c r="Y8" s="78"/>
-      <c r="Z8" s="77"/>
-      <c r="AA8" s="78"/>
-      <c r="AB8" s="77"/>
-      <c r="AC8" s="78"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="83"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="83"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="83"/>
+      <c r="T8" s="82"/>
+      <c r="U8" s="83"/>
+      <c r="V8" s="82"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="83"/>
+      <c r="Z8" s="82"/>
+      <c r="AA8" s="83"/>
+      <c r="AB8" s="82"/>
+      <c r="AC8" s="83"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -1497,10 +1499,10 @@
     <row r="9" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="83"/>
+      <c r="D9" s="88"/>
       <c r="E9" s="9" t="s">
         <v>1</v>
       </c>
@@ -1789,8 +1791,10 @@
       <c r="O16" s="16"/>
       <c r="P16" s="48"/>
       <c r="Q16" s="17"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="16"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="89" t="s">
+        <v>27</v>
+      </c>
       <c r="T16" s="48"/>
       <c r="U16" s="16"/>
       <c r="V16" s="48"/>
@@ -1809,7 +1813,7 @@
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="85"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="70" t="s">
         <v>22</v>
       </c>
@@ -1848,8 +1852,8 @@
     <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="88"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="77"/>
       <c r="E18" s="22" t="s">
         <v>2</v>
       </c>
@@ -1889,7 +1893,7 @@
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="86"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="70" t="s">
         <v>23</v>
       </c>
@@ -1928,8 +1932,8 @@
     <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="88"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="77"/>
       <c r="E20" s="22" t="s">
         <v>2</v>
       </c>
@@ -1967,7 +1971,7 @@
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="86"/>
+      <c r="C21" s="75"/>
       <c r="D21" s="70" t="s">
         <v>24</v>
       </c>
@@ -2006,8 +2010,8 @@
     <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="88"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="77"/>
       <c r="E22" s="31" t="s">
         <v>2</v>
       </c>
@@ -2043,7 +2047,7 @@
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="70"/>
@@ -2225,7 +2229,9 @@
       <c r="Z27" s="49"/>
       <c r="AA27" s="21"/>
       <c r="AB27" s="49"/>
-      <c r="AC27" s="21"/>
+      <c r="AC27" s="90">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="AD27" s="4"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="4"/>
@@ -2234,8 +2240,8 @@
     <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="79"/>
       <c r="E28" s="23" t="s">
         <v>2</v>
       </c>
@@ -2256,7 +2262,9 @@
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="52"/>
-      <c r="S28" s="24"/>
+      <c r="S28" s="68" t="s">
+        <v>28</v>
+      </c>
       <c r="T28" s="52"/>
       <c r="U28" s="24"/>
       <c r="V28" s="52"/>
@@ -2938,14 +2946,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C25:D26"/>
     <mergeCell ref="C27:D28"/>
     <mergeCell ref="AB7:AC8"/>
@@ -2962,6 +2962,14 @@
     <mergeCell ref="L7:M8"/>
     <mergeCell ref="N7:O8"/>
     <mergeCell ref="C9:D10"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Daily commit 21.03.2022 Tag 9
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
+++ b/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\Alles IPA\Git\Cambotmanager-IPA-Maurice-Meier\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF59255-8E1D-4990-8CA5-DD5F23475073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B04B65-CB96-45C2-AAE5-CBD98DDEB4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>07.03.2022</t>
   </si>
@@ -514,17 +514,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -536,8 +525,84 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -553,7 +618,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -566,7 +631,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -578,7 +645,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -590,7 +657,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -598,30 +665,6 @@
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -634,7 +677,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -647,20 +690,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -673,62 +703,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -766,38 +762,38 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -808,21 +804,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -858,8 +839,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D82CD-F568-433E-90D3-FE24E407675F}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,59 +1400,59 @@
     <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="80"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="80" t="s">
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="81"/>
-      <c r="H7" s="80" t="s">
+      <c r="G7" s="76"/>
+      <c r="H7" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="80" t="s">
+      <c r="I7" s="76"/>
+      <c r="J7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="81"/>
-      <c r="L7" s="80" t="s">
+      <c r="K7" s="76"/>
+      <c r="L7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="81"/>
-      <c r="N7" s="80" t="s">
+      <c r="M7" s="76"/>
+      <c r="N7" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="81"/>
-      <c r="P7" s="80" t="s">
+      <c r="O7" s="76"/>
+      <c r="P7" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="80" t="s">
+      <c r="Q7" s="76"/>
+      <c r="R7" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="S7" s="81"/>
-      <c r="T7" s="80" t="s">
+      <c r="S7" s="76"/>
+      <c r="T7" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="81"/>
-      <c r="V7" s="80" t="s">
+      <c r="U7" s="76"/>
+      <c r="V7" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="W7" s="81"/>
-      <c r="X7" s="80" t="s">
+      <c r="W7" s="76"/>
+      <c r="X7" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="81"/>
-      <c r="Z7" s="80" t="s">
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="AA7" s="81"/>
-      <c r="AB7" s="80" t="s">
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="AC7" s="81"/>
+      <c r="AC7" s="76"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
@@ -1464,33 +1461,33 @@
     <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="83"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="82"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="82"/>
-      <c r="U8" s="83"/>
-      <c r="V8" s="82"/>
-      <c r="W8" s="83"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="83"/>
-      <c r="Z8" s="82"/>
-      <c r="AA8" s="83"/>
-      <c r="AB8" s="82"/>
-      <c r="AC8" s="83"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="78"/>
+      <c r="T8" s="77"/>
+      <c r="U8" s="78"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="78"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="78"/>
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="78"/>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="78"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -1499,36 +1496,36 @@
     <row r="9" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="88"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="45"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="47"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="47"/>
+      <c r="L9" s="45"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="47"/>
+      <c r="N9" s="45"/>
       <c r="O9" s="13"/>
-      <c r="P9" s="47"/>
+      <c r="P9" s="45"/>
       <c r="Q9" s="11"/>
-      <c r="R9" s="47"/>
+      <c r="R9" s="45"/>
       <c r="S9" s="13"/>
-      <c r="T9" s="47"/>
+      <c r="T9" s="45"/>
       <c r="U9" s="13"/>
-      <c r="V9" s="47"/>
+      <c r="V9" s="45"/>
       <c r="W9" s="13"/>
-      <c r="X9" s="47"/>
+      <c r="X9" s="45"/>
       <c r="Y9" s="11"/>
-      <c r="Z9" s="47"/>
+      <c r="Z9" s="45"/>
       <c r="AA9" s="13"/>
-      <c r="AB9" s="47"/>
+      <c r="AB9" s="45"/>
       <c r="AC9" s="13"/>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
@@ -1544,30 +1541,30 @@
         <v>2</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="17"/>
-      <c r="J10" s="48"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="60" t="s">
+      <c r="L10" s="58" t="s">
         <v>26</v>
       </c>
       <c r="M10" s="16"/>
-      <c r="N10" s="48"/>
+      <c r="N10" s="46"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="48"/>
+      <c r="P10" s="46"/>
       <c r="Q10" s="17"/>
-      <c r="R10" s="48"/>
+      <c r="R10" s="46"/>
       <c r="S10" s="16"/>
-      <c r="T10" s="48"/>
+      <c r="T10" s="46"/>
       <c r="U10" s="16"/>
-      <c r="V10" s="48"/>
+      <c r="V10" s="46"/>
       <c r="W10" s="16"/>
-      <c r="X10" s="48"/>
+      <c r="X10" s="46"/>
       <c r="Y10" s="17"/>
-      <c r="Z10" s="48"/>
+      <c r="Z10" s="46"/>
       <c r="AA10" s="16"/>
-      <c r="AB10" s="48"/>
+      <c r="AB10" s="46"/>
       <c r="AC10" s="16"/>
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
@@ -1585,28 +1582,28 @@
         <v>1</v>
       </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="49"/>
+      <c r="J11" s="47"/>
       <c r="K11" s="21"/>
-      <c r="L11" s="50"/>
+      <c r="L11" s="48"/>
       <c r="M11" s="19"/>
-      <c r="N11" s="50"/>
+      <c r="N11" s="48"/>
       <c r="O11" s="19"/>
-      <c r="P11" s="50"/>
+      <c r="P11" s="48"/>
       <c r="Q11" s="20"/>
-      <c r="R11" s="50"/>
+      <c r="R11" s="48"/>
       <c r="S11" s="19"/>
-      <c r="T11" s="50"/>
+      <c r="T11" s="48"/>
       <c r="U11" s="19"/>
-      <c r="V11" s="50"/>
+      <c r="V11" s="48"/>
       <c r="W11" s="19"/>
-      <c r="X11" s="50"/>
+      <c r="X11" s="48"/>
       <c r="Y11" s="20"/>
-      <c r="Z11" s="50"/>
+      <c r="Z11" s="48"/>
       <c r="AA11" s="19"/>
-      <c r="AB11" s="50"/>
+      <c r="AB11" s="48"/>
       <c r="AC11" s="19"/>
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
@@ -1622,32 +1619,32 @@
         <v>2</v>
       </c>
       <c r="F12" s="15"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="40" t="s">
+      <c r="G12" s="40"/>
+      <c r="H12" s="38" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="28"/>
-      <c r="J12" s="58" t="s">
+      <c r="J12" s="56" t="s">
         <v>27</v>
       </c>
       <c r="K12" s="16"/>
-      <c r="L12" s="48"/>
+      <c r="L12" s="46"/>
       <c r="M12" s="16"/>
-      <c r="N12" s="48"/>
+      <c r="N12" s="46"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="48"/>
+      <c r="P12" s="46"/>
       <c r="Q12" s="17"/>
-      <c r="R12" s="48"/>
+      <c r="R12" s="46"/>
       <c r="S12" s="16"/>
-      <c r="T12" s="48"/>
+      <c r="T12" s="46"/>
       <c r="U12" s="16"/>
-      <c r="V12" s="48"/>
+      <c r="V12" s="46"/>
       <c r="W12" s="16"/>
-      <c r="X12" s="48"/>
+      <c r="X12" s="46"/>
       <c r="Y12" s="17"/>
-      <c r="Z12" s="48"/>
+      <c r="Z12" s="46"/>
       <c r="AA12" s="16"/>
-      <c r="AB12" s="48"/>
+      <c r="AB12" s="46"/>
       <c r="AC12" s="16"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
@@ -1665,28 +1662,28 @@
         <v>1</v>
       </c>
       <c r="F13" s="12"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="20"/>
-      <c r="J13" s="50"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="19"/>
-      <c r="L13" s="49"/>
+      <c r="L13" s="47"/>
       <c r="M13" s="19"/>
-      <c r="N13" s="50"/>
+      <c r="N13" s="48"/>
       <c r="O13" s="19"/>
-      <c r="P13" s="50"/>
+      <c r="P13" s="48"/>
       <c r="Q13" s="20"/>
-      <c r="R13" s="50"/>
+      <c r="R13" s="48"/>
       <c r="S13" s="19"/>
-      <c r="T13" s="50"/>
+      <c r="T13" s="48"/>
       <c r="U13" s="19"/>
-      <c r="V13" s="50"/>
+      <c r="V13" s="48"/>
       <c r="W13" s="19"/>
-      <c r="X13" s="50"/>
+      <c r="X13" s="48"/>
       <c r="Y13" s="20"/>
-      <c r="Z13" s="50"/>
+      <c r="Z13" s="48"/>
       <c r="AA13" s="19"/>
-      <c r="AB13" s="50"/>
+      <c r="AB13" s="48"/>
       <c r="AC13" s="19"/>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
@@ -1702,30 +1699,30 @@
         <v>2</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="59" t="s">
+      <c r="J14" s="46"/>
+      <c r="K14" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="48"/>
+      <c r="L14" s="46"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="48"/>
+      <c r="N14" s="46"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="48"/>
+      <c r="P14" s="46"/>
       <c r="Q14" s="17"/>
-      <c r="R14" s="48"/>
+      <c r="R14" s="46"/>
       <c r="S14" s="16"/>
-      <c r="T14" s="48"/>
+      <c r="T14" s="46"/>
       <c r="U14" s="16"/>
-      <c r="V14" s="48"/>
+      <c r="V14" s="46"/>
       <c r="W14" s="16"/>
-      <c r="X14" s="48"/>
+      <c r="X14" s="46"/>
       <c r="Y14" s="17"/>
-      <c r="Z14" s="48"/>
+      <c r="Z14" s="46"/>
       <c r="AA14" s="16"/>
-      <c r="AB14" s="48"/>
+      <c r="AB14" s="46"/>
       <c r="AC14" s="16"/>
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
@@ -1743,28 +1740,28 @@
         <v>1</v>
       </c>
       <c r="F15" s="12"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="50"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="48"/>
       <c r="M15" s="21"/>
-      <c r="N15" s="49"/>
+      <c r="N15" s="47"/>
       <c r="O15" s="21"/>
-      <c r="P15" s="49"/>
+      <c r="P15" s="47"/>
       <c r="Q15" s="20"/>
-      <c r="R15" s="49"/>
+      <c r="R15" s="47"/>
       <c r="S15" s="21"/>
-      <c r="T15" s="49"/>
+      <c r="T15" s="47"/>
       <c r="U15" s="21"/>
-      <c r="V15" s="49"/>
+      <c r="V15" s="47"/>
       <c r="W15" s="19"/>
-      <c r="X15" s="50"/>
+      <c r="X15" s="48"/>
       <c r="Y15" s="20"/>
-      <c r="Z15" s="50"/>
+      <c r="Z15" s="48"/>
       <c r="AA15" s="19"/>
-      <c r="AB15" s="50"/>
+      <c r="AB15" s="48"/>
       <c r="AC15" s="19"/>
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
@@ -1780,30 +1777,32 @@
         <v>2</v>
       </c>
       <c r="F16" s="15"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="54"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="52"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="48"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="48"/>
+      <c r="N16" s="46"/>
       <c r="O16" s="16"/>
-      <c r="P16" s="48"/>
+      <c r="P16" s="46"/>
       <c r="Q16" s="17"/>
-      <c r="R16" s="58"/>
-      <c r="S16" s="89" t="s">
+      <c r="R16" s="56"/>
+      <c r="S16" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="48"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="48"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="V16" s="46"/>
       <c r="W16" s="16"/>
-      <c r="X16" s="48"/>
+      <c r="X16" s="46"/>
       <c r="Y16" s="17"/>
-      <c r="Z16" s="48"/>
+      <c r="Z16" s="46"/>
       <c r="AA16" s="16"/>
-      <c r="AB16" s="48"/>
+      <c r="AB16" s="46"/>
       <c r="AC16" s="16"/>
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
@@ -1813,7 +1812,7 @@
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="74"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="70" t="s">
         <v>22</v>
       </c>
@@ -1821,28 +1820,28 @@
         <v>1</v>
       </c>
       <c r="F17" s="12"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
       <c r="I17" s="20"/>
-      <c r="J17" s="50"/>
+      <c r="J17" s="48"/>
       <c r="K17" s="19"/>
-      <c r="L17" s="50"/>
+      <c r="L17" s="48"/>
       <c r="M17" s="21"/>
-      <c r="N17" s="49"/>
+      <c r="N17" s="47"/>
       <c r="O17" s="21"/>
-      <c r="P17" s="49"/>
+      <c r="P17" s="47"/>
       <c r="Q17" s="20"/>
-      <c r="R17" s="50"/>
+      <c r="R17" s="48"/>
       <c r="S17" s="19"/>
-      <c r="T17" s="50"/>
+      <c r="T17" s="48"/>
       <c r="U17" s="19"/>
-      <c r="V17" s="50"/>
+      <c r="V17" s="48"/>
       <c r="W17" s="19"/>
-      <c r="X17" s="50"/>
+      <c r="X17" s="48"/>
       <c r="Y17" s="20"/>
-      <c r="Z17" s="50"/>
+      <c r="Z17" s="48"/>
       <c r="AA17" s="19"/>
-      <c r="AB17" s="50"/>
+      <c r="AB17" s="48"/>
       <c r="AC17" s="19"/>
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
@@ -1852,38 +1851,38 @@
     <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="77"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F18" s="15"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="60" t="s">
+      <c r="J18" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="59"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="60"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="58"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="60" t="s">
+      <c r="P18" s="58" t="s">
         <v>25</v>
       </c>
       <c r="Q18" s="17"/>
-      <c r="R18" s="48"/>
+      <c r="R18" s="46"/>
       <c r="S18" s="16"/>
-      <c r="T18" s="48"/>
+      <c r="T18" s="46"/>
       <c r="U18" s="16"/>
-      <c r="V18" s="48"/>
+      <c r="V18" s="46"/>
       <c r="W18" s="16"/>
-      <c r="X18" s="48"/>
+      <c r="X18" s="46"/>
       <c r="Y18" s="17"/>
-      <c r="Z18" s="48"/>
+      <c r="Z18" s="46"/>
       <c r="AA18" s="16"/>
-      <c r="AB18" s="48"/>
+      <c r="AB18" s="46"/>
       <c r="AC18" s="16"/>
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
@@ -1893,7 +1892,7 @@
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="75"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="70" t="s">
         <v>23</v>
       </c>
@@ -1901,28 +1900,28 @@
         <v>1</v>
       </c>
       <c r="F19" s="12"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="50"/>
+      <c r="J19" s="48"/>
       <c r="K19" s="19"/>
-      <c r="L19" s="50"/>
+      <c r="L19" s="48"/>
       <c r="M19" s="19"/>
-      <c r="N19" s="50"/>
+      <c r="N19" s="48"/>
       <c r="O19" s="19"/>
-      <c r="P19" s="50"/>
+      <c r="P19" s="48"/>
       <c r="Q19" s="20"/>
-      <c r="R19" s="49"/>
+      <c r="R19" s="47"/>
       <c r="S19" s="21"/>
-      <c r="T19" s="50"/>
+      <c r="T19" s="48"/>
       <c r="U19" s="19"/>
-      <c r="V19" s="50"/>
+      <c r="V19" s="48"/>
       <c r="W19" s="19"/>
-      <c r="X19" s="50"/>
+      <c r="X19" s="48"/>
       <c r="Y19" s="20"/>
-      <c r="Z19" s="50"/>
+      <c r="Z19" s="48"/>
       <c r="AA19" s="19"/>
-      <c r="AB19" s="50"/>
+      <c r="AB19" s="48"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
@@ -1932,36 +1931,38 @@
     <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="77"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="88"/>
       <c r="E20" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F20" s="12"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
       <c r="I20" s="20"/>
-      <c r="J20" s="50"/>
+      <c r="J20" s="48"/>
       <c r="K20" s="19"/>
-      <c r="L20" s="50"/>
+      <c r="L20" s="48"/>
       <c r="M20" s="19"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="65"/>
-      <c r="P20" s="66" t="s">
+      <c r="N20" s="48"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="64" t="s">
         <v>29</v>
       </c>
       <c r="Q20" s="20"/>
-      <c r="R20" s="50"/>
+      <c r="R20" s="48"/>
       <c r="S20" s="19"/>
-      <c r="T20" s="50"/>
+      <c r="T20" s="64" t="s">
+        <v>29</v>
+      </c>
       <c r="U20" s="19"/>
-      <c r="V20" s="50"/>
+      <c r="V20" s="48"/>
       <c r="W20" s="19"/>
-      <c r="X20" s="50"/>
+      <c r="X20" s="48"/>
       <c r="Y20" s="20"/>
-      <c r="Z20" s="50"/>
+      <c r="Z20" s="48"/>
       <c r="AA20" s="19"/>
-      <c r="AB20" s="50"/>
+      <c r="AB20" s="48"/>
       <c r="AC20" s="19"/>
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
@@ -1971,7 +1972,7 @@
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="75"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="70" t="s">
         <v>24</v>
       </c>
@@ -1979,30 +1980,30 @@
         <v>1</v>
       </c>
       <c r="F21" s="32"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="34"/>
-      <c r="J21" s="51"/>
+      <c r="J21" s="49"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="51"/>
+      <c r="L21" s="49"/>
       <c r="M21" s="33"/>
-      <c r="N21" s="51"/>
+      <c r="N21" s="49"/>
       <c r="O21" s="33"/>
-      <c r="P21" s="51"/>
+      <c r="P21" s="49"/>
       <c r="Q21" s="34"/>
-      <c r="R21" s="51"/>
+      <c r="R21" s="49"/>
       <c r="S21" s="33"/>
-      <c r="T21" s="53"/>
+      <c r="T21" s="51"/>
       <c r="U21" s="35"/>
-      <c r="V21" s="53"/>
+      <c r="V21" s="51"/>
       <c r="W21" s="33"/>
-      <c r="X21" s="51"/>
+      <c r="X21" s="49"/>
       <c r="Y21" s="34"/>
-      <c r="Z21" s="51"/>
+      <c r="Z21" s="49"/>
       <c r="AA21" s="33"/>
-      <c r="AB21" s="51"/>
-      <c r="AC21" s="36"/>
-      <c r="AD21" s="4"/>
+      <c r="AB21" s="49"/>
+      <c r="AC21" s="91"/>
+      <c r="AD21" s="90"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
@@ -2010,36 +2011,36 @@
     <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="77"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="88"/>
       <c r="E22" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="48"/>
+      <c r="J22" s="46"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="48"/>
+      <c r="L22" s="46"/>
       <c r="M22" s="16"/>
-      <c r="N22" s="48"/>
+      <c r="N22" s="46"/>
       <c r="O22" s="16"/>
-      <c r="P22" s="48"/>
+      <c r="P22" s="46"/>
       <c r="Q22" s="17"/>
-      <c r="R22" s="48"/>
+      <c r="R22" s="46"/>
       <c r="S22" s="16"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="48"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="46"/>
       <c r="W22" s="16"/>
-      <c r="X22" s="48"/>
+      <c r="X22" s="46"/>
       <c r="Y22" s="17"/>
-      <c r="Z22" s="48"/>
+      <c r="Z22" s="46"/>
       <c r="AA22" s="16"/>
-      <c r="AB22" s="48"/>
-      <c r="AC22" s="38"/>
-      <c r="AD22" s="4"/>
+      <c r="AB22" s="46"/>
+      <c r="AC22" s="89"/>
+      <c r="AD22" s="90"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
@@ -2047,7 +2048,7 @@
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="84" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="70"/>
@@ -2055,28 +2056,28 @@
         <v>1</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
       <c r="I23" s="20"/>
-      <c r="J23" s="50"/>
+      <c r="J23" s="48"/>
       <c r="K23" s="19"/>
-      <c r="L23" s="50"/>
+      <c r="L23" s="48"/>
       <c r="M23" s="19"/>
-      <c r="N23" s="50"/>
+      <c r="N23" s="48"/>
       <c r="O23" s="19"/>
-      <c r="P23" s="50"/>
+      <c r="P23" s="48"/>
       <c r="Q23" s="20"/>
-      <c r="R23" s="50"/>
+      <c r="R23" s="48"/>
       <c r="S23" s="19"/>
-      <c r="T23" s="50"/>
+      <c r="T23" s="48"/>
       <c r="U23" s="19"/>
-      <c r="V23" s="50"/>
+      <c r="V23" s="48"/>
       <c r="W23" s="21"/>
-      <c r="X23" s="49"/>
+      <c r="X23" s="47"/>
       <c r="Y23" s="20"/>
-      <c r="Z23" s="50"/>
+      <c r="Z23" s="48"/>
       <c r="AA23" s="19"/>
-      <c r="AB23" s="50"/>
+      <c r="AB23" s="48"/>
       <c r="AC23" s="19"/>
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
@@ -2092,28 +2093,30 @@
         <v>2</v>
       </c>
       <c r="F24" s="15"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="48"/>
+      <c r="J24" s="46"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="48"/>
+      <c r="L24" s="46"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="48"/>
+      <c r="N24" s="46"/>
       <c r="O24" s="16"/>
-      <c r="P24" s="48"/>
+      <c r="P24" s="46"/>
       <c r="Q24" s="17"/>
-      <c r="R24" s="48"/>
+      <c r="R24" s="46"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="48"/>
+      <c r="T24" s="46"/>
       <c r="U24" s="16"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="48"/>
+      <c r="V24" s="46"/>
+      <c r="W24" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="X24" s="46"/>
       <c r="Y24" s="17"/>
-      <c r="Z24" s="48"/>
+      <c r="Z24" s="46"/>
       <c r="AA24" s="16"/>
-      <c r="AB24" s="48"/>
+      <c r="AB24" s="46"/>
       <c r="AC24" s="16"/>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
@@ -2131,28 +2134,28 @@
         <v>1</v>
       </c>
       <c r="F25" s="12"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
       <c r="I25" s="20"/>
-      <c r="J25" s="50"/>
+      <c r="J25" s="48"/>
       <c r="K25" s="19"/>
-      <c r="L25" s="50"/>
+      <c r="L25" s="48"/>
       <c r="M25" s="19"/>
-      <c r="N25" s="50"/>
+      <c r="N25" s="48"/>
       <c r="O25" s="19"/>
-      <c r="P25" s="50"/>
+      <c r="P25" s="48"/>
       <c r="Q25" s="20"/>
-      <c r="R25" s="50"/>
+      <c r="R25" s="48"/>
       <c r="S25" s="19"/>
-      <c r="T25" s="50"/>
+      <c r="T25" s="48"/>
       <c r="U25" s="19"/>
-      <c r="V25" s="50"/>
+      <c r="V25" s="48"/>
       <c r="W25" s="19"/>
-      <c r="X25" s="50"/>
+      <c r="X25" s="48"/>
       <c r="Y25" s="20"/>
-      <c r="Z25" s="49"/>
+      <c r="Z25" s="47"/>
       <c r="AA25" s="21"/>
-      <c r="AB25" s="50"/>
+      <c r="AB25" s="48"/>
       <c r="AC25" s="19"/>
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
@@ -2168,28 +2171,28 @@
         <v>2</v>
       </c>
       <c r="F26" s="15"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
       <c r="I26" s="17"/>
-      <c r="J26" s="48"/>
+      <c r="J26" s="46"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="48"/>
+      <c r="L26" s="46"/>
       <c r="M26" s="16"/>
-      <c r="N26" s="48"/>
+      <c r="N26" s="46"/>
       <c r="O26" s="16"/>
-      <c r="P26" s="48"/>
+      <c r="P26" s="46"/>
       <c r="Q26" s="17"/>
-      <c r="R26" s="48"/>
+      <c r="R26" s="46"/>
       <c r="S26" s="16"/>
-      <c r="T26" s="48"/>
+      <c r="T26" s="46"/>
       <c r="U26" s="16"/>
-      <c r="V26" s="48"/>
+      <c r="V26" s="46"/>
       <c r="W26" s="16"/>
-      <c r="X26" s="48"/>
+      <c r="X26" s="46"/>
       <c r="Y26" s="17"/>
-      <c r="Z26" s="48"/>
+      <c r="Z26" s="46"/>
       <c r="AA26" s="16"/>
-      <c r="AB26" s="48"/>
+      <c r="AB26" s="46"/>
       <c r="AC26" s="16"/>
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
@@ -2207,29 +2210,29 @@
         <v>1</v>
       </c>
       <c r="F27" s="10"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
       <c r="I27" s="20"/>
-      <c r="J27" s="49"/>
+      <c r="J27" s="47"/>
       <c r="K27" s="21"/>
-      <c r="L27" s="49"/>
+      <c r="L27" s="47"/>
       <c r="M27" s="21"/>
-      <c r="N27" s="49"/>
+      <c r="N27" s="47"/>
       <c r="O27" s="21"/>
-      <c r="P27" s="49"/>
+      <c r="P27" s="47"/>
       <c r="Q27" s="20"/>
-      <c r="R27" s="49"/>
+      <c r="R27" s="47"/>
       <c r="S27" s="21"/>
-      <c r="T27" s="49"/>
+      <c r="T27" s="47"/>
       <c r="U27" s="21"/>
-      <c r="V27" s="49"/>
+      <c r="V27" s="47"/>
       <c r="W27" s="21"/>
-      <c r="X27" s="49"/>
+      <c r="X27" s="47"/>
       <c r="Y27" s="20"/>
-      <c r="Z27" s="49"/>
+      <c r="Z27" s="47"/>
       <c r="AA27" s="21"/>
-      <c r="AB27" s="49"/>
-      <c r="AC27" s="90">
+      <c r="AB27" s="47"/>
+      <c r="AC27" s="68">
         <v>0.54166666666666663</v>
       </c>
       <c r="AD27" s="4"/>
@@ -2240,40 +2243,40 @@
     <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="79"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="74"/>
       <c r="E28" s="23" t="s">
         <v>2</v>
       </c>
       <c r="F28" s="27"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="46"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="44"/>
       <c r="I28" s="25"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="68" t="s">
+      <c r="J28" s="50"/>
+      <c r="K28" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="L28" s="52"/>
+      <c r="L28" s="50"/>
       <c r="M28" s="24"/>
-      <c r="N28" s="52"/>
+      <c r="N28" s="50"/>
       <c r="O28" s="24"/>
-      <c r="P28" s="67" t="s">
+      <c r="P28" s="65" t="s">
         <v>25</v>
       </c>
       <c r="Q28" s="25"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="68" t="s">
+      <c r="R28" s="50"/>
+      <c r="S28" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="T28" s="52"/>
+      <c r="T28" s="50"/>
       <c r="U28" s="24"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="52"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="66"/>
+      <c r="X28" s="50"/>
       <c r="Y28" s="25"/>
-      <c r="Z28" s="52"/>
+      <c r="Z28" s="50"/>
       <c r="AA28" s="24"/>
-      <c r="AB28" s="52"/>
+      <c r="AB28" s="50"/>
       <c r="AC28" s="24"/>
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
@@ -2311,7 +2314,7 @@
       <c r="AB29" s="4"/>
       <c r="AC29" s="4"/>
       <c r="AD29" s="4"/>
-      <c r="AE29" s="4"/>
+      <c r="AE29" s="6"/>
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
     </row>
@@ -2436,7 +2439,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="55"/>
+      <c r="P33" s="53"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
@@ -2886,7 +2889,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="57"/>
+      <c r="I46" s="55"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2946,6 +2949,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="C25:D26"/>
     <mergeCell ref="C27:D28"/>
     <mergeCell ref="AB7:AC8"/>
@@ -2962,14 +2973,6 @@
     <mergeCell ref="L7:M8"/>
     <mergeCell ref="N7:O8"/>
     <mergeCell ref="C9:D10"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Daily Commmit Tag 11 24.03.2022
</commit_message>
<xml_diff>
--- a/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
+++ b/Dokumentation/ZeitPlan IPA Maurice Meier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maurice\Desktop\Alles IPA\Git\Cambotmanager-IPA-Maurice-Meier\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B04B65-CB96-45C2-AAE5-CBD98DDEB4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADC97F5-E4BF-4391-A19B-194121925F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
+    <workbookView xWindow="13932" yWindow="2028" windowWidth="17280" windowHeight="9024" xr2:uid="{257C4A67-2D95-420C-B821-9BE4F41869F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>07.03.2022</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>Tätigkeit</t>
+  </si>
+  <si>
+    <t>Montag</t>
+  </si>
+  <si>
+    <t>Mittwoch</t>
+  </si>
+  <si>
+    <t>Donnerstag</t>
+  </si>
+  <si>
+    <t>Freitag</t>
   </si>
 </sst>
 </file>
@@ -219,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -531,19 +543,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -724,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -762,38 +761,58 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -815,22 +834,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -842,24 +846,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -880,7 +883,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1178,16 +1181,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D82CD-F568-433E-90D3-FE24E407675F}">
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE29" sqref="AE29"/>
+    <sheetView tabSelected="1" topLeftCell="V5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="20.42578125" customWidth="1"/>
+    <col min="3" max="4" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -1222,7 +1225,7 @@
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1257,7 +1260,7 @@
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1292,7 +1295,7 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1327,7 +1330,7 @@
       <c r="AF4" s="4"/>
       <c r="AG4" s="4"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1362,7 +1365,7 @@
       <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
     </row>
-    <row r="6" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1397,842 +1400,872 @@
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
     </row>
-    <row r="7" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="75" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="75" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="76"/>
-      <c r="N7" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" s="76"/>
-      <c r="P7" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="75" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7" s="76"/>
-      <c r="T7" s="75" t="s">
-        <v>16</v>
-      </c>
-      <c r="U7" s="76"/>
-      <c r="V7" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="W7" s="76"/>
-      <c r="X7" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y7" s="76"/>
-      <c r="Z7" s="75" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA7" s="76"/>
-      <c r="AB7" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC7" s="76"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="72"/>
+      <c r="H7" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="72"/>
+      <c r="J7" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="72"/>
+      <c r="L7" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="72"/>
+      <c r="N7" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="72"/>
+      <c r="P7" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" s="72"/>
+      <c r="T7" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="72"/>
+      <c r="V7" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="W7" s="72"/>
+      <c r="X7" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y7" s="72"/>
+      <c r="Z7" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA7" s="72"/>
+      <c r="AB7" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC7" s="72"/>
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
     </row>
-    <row r="8" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="78"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="78"/>
-      <c r="T8" s="77"/>
-      <c r="U8" s="78"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="78"/>
-      <c r="X8" s="77"/>
-      <c r="Y8" s="78"/>
-      <c r="Z8" s="77"/>
-      <c r="AA8" s="78"/>
-      <c r="AB8" s="77"/>
-      <c r="AC8" s="78"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="76"/>
+      <c r="H8" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="74"/>
+      <c r="J8" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="74"/>
+      <c r="L8" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="74"/>
+      <c r="N8" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="74"/>
+      <c r="P8" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="74"/>
+      <c r="T8" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="U8" s="74"/>
+      <c r="V8" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="W8" s="74"/>
+      <c r="X8" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC8" s="74"/>
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
       <c r="AG8" s="4"/>
     </row>
-    <row r="9" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="83"/>
+      <c r="D9" s="86"/>
       <c r="E9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="43"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="45"/>
+      <c r="J9" s="44"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="45"/>
+      <c r="L9" s="44"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="45"/>
+      <c r="N9" s="44"/>
       <c r="O9" s="13"/>
-      <c r="P9" s="45"/>
+      <c r="P9" s="44"/>
       <c r="Q9" s="11"/>
-      <c r="R9" s="45"/>
+      <c r="R9" s="44"/>
       <c r="S9" s="13"/>
-      <c r="T9" s="45"/>
+      <c r="T9" s="44"/>
       <c r="U9" s="13"/>
-      <c r="V9" s="45"/>
+      <c r="V9" s="44"/>
       <c r="W9" s="13"/>
-      <c r="X9" s="45"/>
+      <c r="X9" s="44"/>
       <c r="Y9" s="11"/>
-      <c r="Z9" s="45"/>
+      <c r="Z9" s="44"/>
       <c r="AA9" s="13"/>
-      <c r="AB9" s="45"/>
+      <c r="AB9" s="44"/>
       <c r="AC9" s="13"/>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
       <c r="AG9" s="4"/>
     </row>
-    <row r="10" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="72"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="80"/>
       <c r="E10" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="17"/>
-      <c r="J10" s="46"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="58" t="s">
+      <c r="L10" s="57" t="s">
         <v>26</v>
       </c>
       <c r="M10" s="16"/>
-      <c r="N10" s="46"/>
+      <c r="N10" s="45"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="46"/>
+      <c r="P10" s="45"/>
       <c r="Q10" s="17"/>
-      <c r="R10" s="46"/>
+      <c r="R10" s="45"/>
       <c r="S10" s="16"/>
-      <c r="T10" s="46"/>
+      <c r="T10" s="45"/>
       <c r="U10" s="16"/>
-      <c r="V10" s="46"/>
+      <c r="V10" s="45"/>
       <c r="W10" s="16"/>
-      <c r="X10" s="46"/>
+      <c r="X10" s="45"/>
       <c r="Y10" s="17"/>
-      <c r="Z10" s="46"/>
+      <c r="Z10" s="45"/>
       <c r="AA10" s="16"/>
-      <c r="AB10" s="46"/>
+      <c r="AB10" s="45"/>
       <c r="AC10" s="16"/>
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
       <c r="AG10" s="4"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="70"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="47"/>
+      <c r="J11" s="46"/>
       <c r="K11" s="21"/>
-      <c r="L11" s="48"/>
+      <c r="L11" s="47"/>
       <c r="M11" s="19"/>
-      <c r="N11" s="48"/>
+      <c r="N11" s="47"/>
       <c r="O11" s="19"/>
-      <c r="P11" s="48"/>
+      <c r="P11" s="47"/>
       <c r="Q11" s="20"/>
-      <c r="R11" s="48"/>
+      <c r="R11" s="47"/>
       <c r="S11" s="19"/>
-      <c r="T11" s="48"/>
+      <c r="T11" s="47"/>
       <c r="U11" s="19"/>
-      <c r="V11" s="48"/>
+      <c r="V11" s="47"/>
       <c r="W11" s="19"/>
-      <c r="X11" s="48"/>
+      <c r="X11" s="47"/>
       <c r="Y11" s="20"/>
-      <c r="Z11" s="48"/>
+      <c r="Z11" s="47"/>
       <c r="AA11" s="19"/>
-      <c r="AB11" s="48"/>
+      <c r="AB11" s="47"/>
       <c r="AC11" s="19"/>
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
       <c r="AG11" s="4"/>
     </row>
-    <row r="12" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="72"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="80"/>
       <c r="E12" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="15"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="38" t="s">
+      <c r="G12" s="39"/>
+      <c r="H12" s="37" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="28"/>
-      <c r="J12" s="56" t="s">
+      <c r="J12" s="55" t="s">
         <v>27</v>
       </c>
       <c r="K12" s="16"/>
-      <c r="L12" s="46"/>
+      <c r="L12" s="45"/>
       <c r="M12" s="16"/>
-      <c r="N12" s="46"/>
+      <c r="N12" s="45"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="46"/>
+      <c r="P12" s="45"/>
       <c r="Q12" s="17"/>
-      <c r="R12" s="46"/>
+      <c r="R12" s="45"/>
       <c r="S12" s="16"/>
-      <c r="T12" s="46"/>
+      <c r="T12" s="45"/>
       <c r="U12" s="16"/>
-      <c r="V12" s="46"/>
+      <c r="V12" s="45"/>
       <c r="W12" s="16"/>
-      <c r="X12" s="46"/>
+      <c r="X12" s="45"/>
       <c r="Y12" s="17"/>
-      <c r="Z12" s="46"/>
+      <c r="Z12" s="45"/>
       <c r="AA12" s="16"/>
-      <c r="AB12" s="46"/>
+      <c r="AB12" s="45"/>
       <c r="AC12" s="16"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="70"/>
+      <c r="D13" s="78"/>
       <c r="E13" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="12"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="20"/>
-      <c r="J13" s="48"/>
+      <c r="J13" s="47"/>
       <c r="K13" s="19"/>
-      <c r="L13" s="47"/>
+      <c r="L13" s="46"/>
       <c r="M13" s="19"/>
-      <c r="N13" s="48"/>
+      <c r="N13" s="47"/>
       <c r="O13" s="19"/>
-      <c r="P13" s="48"/>
+      <c r="P13" s="47"/>
       <c r="Q13" s="20"/>
-      <c r="R13" s="48"/>
+      <c r="R13" s="47"/>
       <c r="S13" s="19"/>
-      <c r="T13" s="48"/>
+      <c r="T13" s="47"/>
       <c r="U13" s="19"/>
-      <c r="V13" s="48"/>
+      <c r="V13" s="47"/>
       <c r="W13" s="19"/>
-      <c r="X13" s="48"/>
+      <c r="X13" s="47"/>
       <c r="Y13" s="20"/>
-      <c r="Z13" s="48"/>
+      <c r="Z13" s="47"/>
       <c r="AA13" s="19"/>
-      <c r="AB13" s="48"/>
+      <c r="AB13" s="47"/>
       <c r="AC13" s="19"/>
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
     </row>
-    <row r="14" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="72"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="80"/>
       <c r="E14" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="57" t="s">
+      <c r="J14" s="45"/>
+      <c r="K14" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="46"/>
+      <c r="L14" s="45"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="46"/>
+      <c r="N14" s="45"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="46"/>
+      <c r="P14" s="45"/>
       <c r="Q14" s="17"/>
-      <c r="R14" s="46"/>
+      <c r="R14" s="45"/>
       <c r="S14" s="16"/>
-      <c r="T14" s="46"/>
+      <c r="T14" s="45"/>
       <c r="U14" s="16"/>
-      <c r="V14" s="46"/>
+      <c r="V14" s="45"/>
       <c r="W14" s="16"/>
-      <c r="X14" s="46"/>
+      <c r="X14" s="45"/>
       <c r="Y14" s="17"/>
-      <c r="Z14" s="46"/>
+      <c r="Z14" s="45"/>
       <c r="AA14" s="16"/>
-      <c r="AB14" s="46"/>
+      <c r="AB14" s="45"/>
       <c r="AC14" s="16"/>
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
       <c r="AG14" s="4"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="70"/>
+      <c r="D15" s="78"/>
       <c r="E15" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="12"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="20"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="48"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="47"/>
       <c r="M15" s="21"/>
-      <c r="N15" s="47"/>
+      <c r="N15" s="46"/>
       <c r="O15" s="21"/>
-      <c r="P15" s="47"/>
+      <c r="P15" s="46"/>
       <c r="Q15" s="20"/>
-      <c r="R15" s="47"/>
+      <c r="R15" s="46"/>
       <c r="S15" s="21"/>
-      <c r="T15" s="47"/>
+      <c r="T15" s="46"/>
       <c r="U15" s="21"/>
-      <c r="V15" s="47"/>
+      <c r="V15" s="46"/>
       <c r="W15" s="19"/>
-      <c r="X15" s="48"/>
+      <c r="X15" s="47"/>
       <c r="Y15" s="20"/>
-      <c r="Z15" s="48"/>
+      <c r="Z15" s="47"/>
       <c r="AA15" s="19"/>
-      <c r="AB15" s="48"/>
+      <c r="AB15" s="47"/>
       <c r="AC15" s="19"/>
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
       <c r="AG15" s="4"/>
     </row>
-    <row r="16" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="72"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="80"/>
       <c r="E16" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="15"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="52"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="46"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="45"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="46"/>
+      <c r="N16" s="45"/>
       <c r="O16" s="16"/>
-      <c r="P16" s="46"/>
+      <c r="P16" s="45"/>
       <c r="Q16" s="17"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="67" t="s">
+      <c r="R16" s="55"/>
+      <c r="S16" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="T16" s="46"/>
-      <c r="U16" s="67" t="s">
+      <c r="T16" s="45"/>
+      <c r="U16" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="V16" s="46"/>
+      <c r="V16" s="45"/>
       <c r="W16" s="16"/>
-      <c r="X16" s="46"/>
+      <c r="X16" s="57" t="s">
+        <v>25</v>
+      </c>
       <c r="Y16" s="17"/>
-      <c r="Z16" s="46"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="46"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB16" s="45"/>
       <c r="AC16" s="16"/>
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
       <c r="AG16" s="4"/>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="70" t="s">
+      <c r="C17" s="88"/>
+      <c r="D17" s="78" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="12"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="20"/>
-      <c r="J17" s="48"/>
+      <c r="J17" s="47"/>
       <c r="K17" s="19"/>
-      <c r="L17" s="48"/>
+      <c r="L17" s="47"/>
       <c r="M17" s="21"/>
-      <c r="N17" s="47"/>
+      <c r="N17" s="46"/>
       <c r="O17" s="21"/>
-      <c r="P17" s="47"/>
+      <c r="P17" s="46"/>
       <c r="Q17" s="20"/>
-      <c r="R17" s="48"/>
+      <c r="R17" s="47"/>
       <c r="S17" s="19"/>
-      <c r="T17" s="48"/>
+      <c r="T17" s="47"/>
       <c r="U17" s="19"/>
-      <c r="V17" s="48"/>
+      <c r="V17" s="47"/>
       <c r="W17" s="19"/>
-      <c r="X17" s="48"/>
+      <c r="X17" s="47"/>
       <c r="Y17" s="20"/>
-      <c r="Z17" s="48"/>
+      <c r="Z17" s="47"/>
       <c r="AA17" s="19"/>
-      <c r="AB17" s="48"/>
+      <c r="AB17" s="47"/>
       <c r="AC17" s="19"/>
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
     </row>
-    <row r="18" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="91"/>
       <c r="E18" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F18" s="15"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="58" t="s">
+      <c r="J18" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="57"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="58"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="57"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="58" t="s">
+      <c r="P18" s="57" t="s">
         <v>25</v>
       </c>
       <c r="Q18" s="17"/>
-      <c r="R18" s="46"/>
+      <c r="R18" s="45"/>
       <c r="S18" s="16"/>
-      <c r="T18" s="46"/>
+      <c r="T18" s="45"/>
       <c r="U18" s="16"/>
-      <c r="V18" s="46"/>
+      <c r="V18" s="45"/>
       <c r="W18" s="16"/>
-      <c r="X18" s="46"/>
+      <c r="X18" s="45"/>
       <c r="Y18" s="17"/>
-      <c r="Z18" s="46"/>
+      <c r="Z18" s="45"/>
       <c r="AA18" s="16"/>
-      <c r="AB18" s="46"/>
+      <c r="AB18" s="45"/>
       <c r="AC18" s="16"/>
       <c r="AD18" s="4"/>
       <c r="AE18" s="4"/>
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="70" t="s">
+      <c r="C19" s="89"/>
+      <c r="D19" s="78" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="12"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="48"/>
+      <c r="J19" s="47"/>
       <c r="K19" s="19"/>
-      <c r="L19" s="48"/>
+      <c r="L19" s="47"/>
       <c r="M19" s="19"/>
-      <c r="N19" s="48"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="19"/>
-      <c r="P19" s="48"/>
+      <c r="P19" s="47"/>
       <c r="Q19" s="20"/>
-      <c r="R19" s="47"/>
+      <c r="R19" s="46"/>
       <c r="S19" s="21"/>
-      <c r="T19" s="48"/>
+      <c r="T19" s="47"/>
       <c r="U19" s="19"/>
-      <c r="V19" s="48"/>
+      <c r="V19" s="47"/>
       <c r="W19" s="19"/>
-      <c r="X19" s="48"/>
+      <c r="X19" s="47"/>
       <c r="Y19" s="20"/>
-      <c r="Z19" s="48"/>
+      <c r="Z19" s="47"/>
       <c r="AA19" s="19"/>
-      <c r="AB19" s="48"/>
+      <c r="AB19" s="47"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="4"/>
       <c r="AE19" s="4"/>
       <c r="AF19" s="4"/>
       <c r="AG19" s="4"/>
     </row>
-    <row r="20" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="88"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="91"/>
       <c r="E20" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F20" s="12"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
       <c r="I20" s="20"/>
-      <c r="J20" s="48"/>
+      <c r="J20" s="47"/>
       <c r="K20" s="19"/>
-      <c r="L20" s="48"/>
+      <c r="L20" s="47"/>
       <c r="M20" s="19"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="64" t="s">
+      <c r="N20" s="47"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="63" t="s">
         <v>29</v>
       </c>
       <c r="Q20" s="20"/>
-      <c r="R20" s="48"/>
+      <c r="R20" s="47"/>
       <c r="S20" s="19"/>
-      <c r="T20" s="64" t="s">
+      <c r="T20" s="63" t="s">
         <v>29</v>
       </c>
       <c r="U20" s="19"/>
-      <c r="V20" s="48"/>
+      <c r="V20" s="47"/>
       <c r="W20" s="19"/>
-      <c r="X20" s="48"/>
+      <c r="X20" s="47"/>
       <c r="Y20" s="20"/>
-      <c r="Z20" s="48"/>
+      <c r="Z20" s="47"/>
       <c r="AA20" s="19"/>
-      <c r="AB20" s="48"/>
+      <c r="AB20" s="47"/>
       <c r="AC20" s="19"/>
       <c r="AD20" s="4"/>
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
       <c r="AG20" s="4"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="70" t="s">
+      <c r="C21" s="89"/>
+      <c r="D21" s="78" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="30" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="32"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
       <c r="I21" s="34"/>
-      <c r="J21" s="49"/>
+      <c r="J21" s="48"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="49"/>
+      <c r="L21" s="48"/>
       <c r="M21" s="33"/>
-      <c r="N21" s="49"/>
+      <c r="N21" s="48"/>
       <c r="O21" s="33"/>
-      <c r="P21" s="49"/>
+      <c r="P21" s="48"/>
       <c r="Q21" s="34"/>
-      <c r="R21" s="49"/>
+      <c r="R21" s="48"/>
       <c r="S21" s="33"/>
-      <c r="T21" s="51"/>
+      <c r="T21" s="50"/>
       <c r="U21" s="35"/>
-      <c r="V21" s="51"/>
+      <c r="V21" s="50"/>
       <c r="W21" s="33"/>
-      <c r="X21" s="49"/>
+      <c r="X21" s="48"/>
       <c r="Y21" s="34"/>
-      <c r="Z21" s="49"/>
+      <c r="Z21" s="48"/>
       <c r="AA21" s="33"/>
-      <c r="AB21" s="49"/>
-      <c r="AC21" s="91"/>
-      <c r="AD21" s="90"/>
+      <c r="AB21" s="48"/>
+      <c r="AC21" s="70"/>
+      <c r="AD21" s="69"/>
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
     </row>
-    <row r="22" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="88"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91"/>
       <c r="E22" s="31" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="36"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="46"/>
+      <c r="J22" s="45"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="46"/>
+      <c r="L22" s="45"/>
       <c r="M22" s="16"/>
-      <c r="N22" s="46"/>
+      <c r="N22" s="45"/>
       <c r="O22" s="16"/>
-      <c r="P22" s="46"/>
+      <c r="P22" s="45"/>
       <c r="Q22" s="17"/>
-      <c r="R22" s="46"/>
+      <c r="R22" s="45"/>
       <c r="S22" s="16"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="57"/>
-      <c r="V22" s="46"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="56"/>
+      <c r="V22" s="45"/>
       <c r="W22" s="16"/>
-      <c r="X22" s="46"/>
+      <c r="X22" s="45"/>
       <c r="Y22" s="17"/>
-      <c r="Z22" s="46"/>
+      <c r="Z22" s="45"/>
       <c r="AA22" s="16"/>
-      <c r="AB22" s="46"/>
-      <c r="AC22" s="89"/>
-      <c r="AD22" s="90"/>
+      <c r="AB22" s="45"/>
+      <c r="AC22" s="68"/>
+      <c r="AD22" s="69"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="4"/>
       <c r="AG22" s="4"/>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="70"/>
+      <c r="D23" s="78"/>
       <c r="E23" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
       <c r="I23" s="20"/>
-      <c r="J23" s="48"/>
+      <c r="J23" s="47"/>
       <c r="K23" s="19"/>
-      <c r="L23" s="48"/>
+      <c r="L23" s="47"/>
       <c r="M23" s="19"/>
-      <c r="N23" s="48"/>
+      <c r="N23" s="47"/>
       <c r="O23" s="19"/>
-      <c r="P23" s="48"/>
+      <c r="P23" s="47"/>
       <c r="Q23" s="20"/>
-      <c r="R23" s="48"/>
+      <c r="R23" s="47"/>
       <c r="S23" s="19"/>
-      <c r="T23" s="48"/>
+      <c r="T23" s="47"/>
       <c r="U23" s="19"/>
-      <c r="V23" s="48"/>
+      <c r="V23" s="47"/>
       <c r="W23" s="21"/>
-      <c r="X23" s="47"/>
+      <c r="X23" s="46"/>
       <c r="Y23" s="20"/>
-      <c r="Z23" s="48"/>
+      <c r="Z23" s="47"/>
       <c r="AA23" s="19"/>
-      <c r="AB23" s="48"/>
+      <c r="AB23" s="47"/>
       <c r="AC23" s="19"/>
       <c r="AD23" s="4"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4"/>
     </row>
-    <row r="24" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="72"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="80"/>
       <c r="E24" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F24" s="15"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="46"/>
+      <c r="J24" s="45"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="46"/>
+      <c r="L24" s="45"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="46"/>
+      <c r="N24" s="45"/>
       <c r="O24" s="16"/>
-      <c r="P24" s="46"/>
+      <c r="P24" s="45"/>
       <c r="Q24" s="17"/>
-      <c r="R24" s="46"/>
+      <c r="R24" s="45"/>
       <c r="S24" s="16"/>
-      <c r="T24" s="46"/>
+      <c r="T24" s="45"/>
       <c r="U24" s="16"/>
-      <c r="V24" s="46"/>
-      <c r="W24" s="57" t="s">
+      <c r="V24" s="45"/>
+      <c r="W24" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="X24" s="46"/>
+      <c r="X24" s="57" t="s">
+        <v>25</v>
+      </c>
       <c r="Y24" s="17"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="16"/>
-      <c r="AB24" s="46"/>
+      <c r="Z24" s="45"/>
+      <c r="AA24" s="56"/>
+      <c r="AB24" s="45"/>
       <c r="AC24" s="16"/>
       <c r="AD24" s="4"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
       <c r="AG24" s="4"/>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="69" t="s">
+      <c r="C25" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="70"/>
+      <c r="D25" s="78"/>
       <c r="E25" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="12"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
       <c r="I25" s="20"/>
-      <c r="J25" s="48"/>
+      <c r="J25" s="47"/>
       <c r="K25" s="19"/>
-      <c r="L25" s="48"/>
+      <c r="L25" s="47"/>
       <c r="M25" s="19"/>
-      <c r="N25" s="48"/>
+      <c r="N25" s="47"/>
       <c r="O25" s="19"/>
-      <c r="P25" s="48"/>
+      <c r="P25" s="47"/>
       <c r="Q25" s="20"/>
-      <c r="R25" s="48"/>
+      <c r="R25" s="47"/>
       <c r="S25" s="19"/>
-      <c r="T25" s="48"/>
+      <c r="T25" s="47"/>
       <c r="U25" s="19"/>
-      <c r="V25" s="48"/>
+      <c r="V25" s="47"/>
       <c r="W25" s="19"/>
-      <c r="X25" s="48"/>
+      <c r="X25" s="47"/>
       <c r="Y25" s="20"/>
-      <c r="Z25" s="47"/>
+      <c r="Z25" s="46"/>
       <c r="AA25" s="21"/>
-      <c r="AB25" s="48"/>
+      <c r="AB25" s="47"/>
       <c r="AC25" s="19"/>
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="4"/>
       <c r="AG25" s="4"/>
     </row>
-    <row r="26" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="72"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="80"/>
       <c r="E26" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F26" s="15"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
       <c r="I26" s="17"/>
-      <c r="J26" s="46"/>
+      <c r="J26" s="45"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="46"/>
+      <c r="L26" s="45"/>
       <c r="M26" s="16"/>
-      <c r="N26" s="46"/>
+      <c r="N26" s="45"/>
       <c r="O26" s="16"/>
-      <c r="P26" s="46"/>
+      <c r="P26" s="45"/>
       <c r="Q26" s="17"/>
-      <c r="R26" s="46"/>
+      <c r="R26" s="45"/>
       <c r="S26" s="16"/>
-      <c r="T26" s="46"/>
+      <c r="T26" s="45"/>
       <c r="U26" s="16"/>
-      <c r="V26" s="46"/>
+      <c r="V26" s="45"/>
       <c r="W26" s="16"/>
-      <c r="X26" s="46"/>
+      <c r="X26" s="45"/>
       <c r="Y26" s="17"/>
-      <c r="Z26" s="46"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="46"/>
+      <c r="Z26" s="57"/>
+      <c r="AA26" s="93"/>
+      <c r="AB26" s="45"/>
       <c r="AC26" s="16"/>
       <c r="AD26" s="4"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
       <c r="AG26" s="4"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="70"/>
+      <c r="D27" s="78"/>
       <c r="E27" s="18" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="10"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
       <c r="I27" s="20"/>
-      <c r="J27" s="47"/>
+      <c r="J27" s="46"/>
       <c r="K27" s="21"/>
-      <c r="L27" s="47"/>
+      <c r="L27" s="46"/>
       <c r="M27" s="21"/>
-      <c r="N27" s="47"/>
+      <c r="N27" s="46"/>
       <c r="O27" s="21"/>
-      <c r="P27" s="47"/>
+      <c r="P27" s="46"/>
       <c r="Q27" s="20"/>
-      <c r="R27" s="47"/>
+      <c r="R27" s="46"/>
       <c r="S27" s="21"/>
-      <c r="T27" s="47"/>
+      <c r="T27" s="46"/>
       <c r="U27" s="21"/>
-      <c r="V27" s="47"/>
+      <c r="V27" s="46"/>
       <c r="W27" s="21"/>
-      <c r="X27" s="47"/>
+      <c r="X27" s="46"/>
       <c r="Y27" s="20"/>
-      <c r="Z27" s="47"/>
+      <c r="Z27" s="46"/>
       <c r="AA27" s="21"/>
-      <c r="AB27" s="47"/>
-      <c r="AC27" s="68">
+      <c r="AB27" s="46"/>
+      <c r="AC27" s="67">
         <v>0.54166666666666663</v>
       </c>
       <c r="AD27" s="4"/>
@@ -2240,50 +2273,54 @@
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
     </row>
-    <row r="28" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="23" t="s">
         <v>2</v>
       </c>
       <c r="F28" s="27"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="44"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="43"/>
       <c r="I28" s="25"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="66" t="s">
+      <c r="J28" s="49"/>
+      <c r="K28" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="L28" s="50"/>
+      <c r="L28" s="49"/>
       <c r="M28" s="24"/>
-      <c r="N28" s="50"/>
+      <c r="N28" s="49"/>
       <c r="O28" s="24"/>
-      <c r="P28" s="65" t="s">
+      <c r="P28" s="64" t="s">
         <v>25</v>
       </c>
       <c r="Q28" s="25"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="66" t="s">
+      <c r="R28" s="49"/>
+      <c r="S28" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="T28" s="50"/>
+      <c r="T28" s="49"/>
       <c r="U28" s="24"/>
-      <c r="V28" s="65"/>
-      <c r="W28" s="66"/>
-      <c r="X28" s="50"/>
+      <c r="V28" s="64"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="92" t="s">
+        <v>29</v>
+      </c>
       <c r="Y28" s="25"/>
-      <c r="Z28" s="50"/>
-      <c r="AA28" s="24"/>
-      <c r="AB28" s="50"/>
+      <c r="Z28" s="64"/>
+      <c r="AA28" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB28" s="64"/>
       <c r="AC28" s="24"/>
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
       <c r="AF28" s="4"/>
       <c r="AG28" s="4"/>
     </row>
-    <row r="29" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2318,7 +2355,7 @@
       <c r="AF29" s="4"/>
       <c r="AG29" s="4"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2353,7 +2390,7 @@
       <c r="AF30" s="4"/>
       <c r="AG30" s="4"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2388,7 +2425,7 @@
       <c r="AF31" s="4"/>
       <c r="AG31" s="4"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2423,7 +2460,7 @@
       <c r="AF32" s="4"/>
       <c r="AG32" s="4"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2439,7 +2476,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="53"/>
+      <c r="P33" s="52"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
@@ -2458,7 +2495,7 @@
       <c r="AF33" s="4"/>
       <c r="AG33" s="4"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2499,7 +2536,7 @@
       <c r="AF34" s="4"/>
       <c r="AG34" s="4"/>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2534,7 +2571,7 @@
       <c r="AF35" s="4"/>
       <c r="AG35" s="4"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2569,7 +2606,7 @@
       <c r="AF36" s="4"/>
       <c r="AG36" s="4"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2604,7 +2641,7 @@
       <c r="AF37" s="4"/>
       <c r="AG37" s="4"/>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2639,7 +2676,7 @@
       <c r="AF38" s="4"/>
       <c r="AG38" s="4"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2674,7 +2711,7 @@
       <c r="AF39" s="4"/>
       <c r="AG39" s="4"/>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2709,7 +2746,7 @@
       <c r="AF40" s="4"/>
       <c r="AG40" s="4"/>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2744,7 +2781,7 @@
       <c r="AF41" s="4"/>
       <c r="AG41" s="4"/>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2779,7 +2816,7 @@
       <c r="AF42" s="4"/>
       <c r="AG42" s="4"/>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="3"/>
@@ -2814,7 +2851,7 @@
       <c r="AF43" s="4"/>
       <c r="AG43" s="4"/>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="3"/>
@@ -2849,7 +2886,7 @@
       <c r="AF44" s="4"/>
       <c r="AG44" s="4"/>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -2882,14 +2919,14 @@
       <c r="AF45" s="4"/>
       <c r="AG45" s="4"/>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="55"/>
+      <c r="I46" s="54"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2898,7 +2935,7 @@
       <c r="AF46" s="4"/>
       <c r="AG46" s="4"/>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -2911,7 +2948,7 @@
       <c r="L47" s="1"/>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2923,7 +2960,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -2935,7 +2972,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2948,7 +2985,11 @@
       <c r="L50" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="36">
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="C9:D10"/>
     <mergeCell ref="C11:D12"/>
     <mergeCell ref="C13:D14"/>
     <mergeCell ref="C15:D16"/>
@@ -2957,22 +2998,30 @@
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D21:D22"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="AB7:AC8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="V7:W8"/>
-    <mergeCell ref="X7:Y8"/>
-    <mergeCell ref="Z7:AA8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="H7:I8"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="L7:M8"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="AB8:AC8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>